<commit_message>
user excel sheet issue fix
</commit_message>
<xml_diff>
--- a/public/assests/Users.xlsx
+++ b/public/assests/Users.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rudrakshchavda/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rudrakshchavda/Desktop/office/Theba1/ThibaIngoziAdmin/public/assests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AB0B7A-4AFE-8C4B-AB21-917EBB359661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC356912-ACFA-AF46-9B27-482C20756618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>email</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>company_name</t>
-  </si>
-  <si>
-    <t>passport_no</t>
   </si>
   <si>
     <t>John</t>
@@ -366,7 +363,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -406,9 +403,6 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
@@ -422,16 +416,16 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1">
         <v>123</v>
@@ -443,11 +437,9 @@
         <v>7894561230</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
-      <c r="I3" s="1">
-        <v>232455</v>
-      </c>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>

</xml_diff>